<commit_message>
standardize duff and litter data for anova
</commit_message>
<xml_diff>
--- a/input/data_1-raw/FOR_Fuels_MorganANOVA.xlsx
+++ b/input/data_1-raw/FOR_Fuels_MorganANOVA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgray/Documents/GitHub/rxf_veg-plots/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgray/Documents/GitHub/woody-fuels/input/data_1-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC57B72-F739-6144-AFE9-6A5137F27724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D59FE3-61D4-D64D-8343-A4DBCD464634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30280" windowHeight="20780" xr2:uid="{A10E1E61-F7FD-4AA7-99BF-399F8AF932AF}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>